<commit_message>
crud operation ObjectController add
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/dodatok_01-04-2021_18_28_30.xlsx
+++ b/src/main/resources/excel/dodatok_01-04-2021_18_28_30.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="557">
   <si>
     <t>№</t>
   </si>
@@ -1689,6 +1689,12 @@
   </si>
   <si>
     <t>РАДІОСТАНЦІЯ "KENWOOD" TK-90 (КОРОТКОХВИЛЬОВОГО ДІАПАЗОНУ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комутатори </t>
+  </si>
+  <si>
+    <t>cisco 515-px</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1702,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1821,6 +1827,91 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -2130,7 +2221,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="justify" wrapText="1"/>
@@ -2351,6 +2442,57 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="23" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal_Sheet1" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -37270,7 +37412,7 @@
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="91" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="37"/>
@@ -37848,7 +37990,7 @@
     </row>
     <row r="75" spans="1:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="44"/>
-      <c r="B75" s="74" t="s">
+      <c r="B75" s="91" t="s">
         <v>120</v>
       </c>
       <c r="C75" s="37"/>
@@ -38196,7 +38338,7 @@
     </row>
     <row r="110" spans="1:4" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="44"/>
-      <c r="B110" s="74" t="s">
+      <c r="B110" s="91" t="s">
         <v>155</v>
       </c>
       <c r="C110" s="37"/>
@@ -38224,7 +38366,7 @@
     </row>
     <row r="113" spans="1:4" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="44"/>
-      <c r="B113" s="74" t="s">
+      <c r="B113" s="91" t="s">
         <v>158</v>
       </c>
       <c r="C113" s="37"/>
@@ -38242,7 +38384,7 @@
     </row>
     <row r="115" spans="1:4" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="44"/>
-      <c r="B115" s="74" t="s">
+      <c r="B115" s="91" t="s">
         <v>160</v>
       </c>
       <c r="C115" s="37"/>
@@ -38260,7 +38402,7 @@
     </row>
     <row r="117" spans="1:4" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="44"/>
-      <c r="B117" s="74" t="s">
+      <c r="B117" s="91" t="s">
         <v>162</v>
       </c>
       <c r="C117" s="37"/>
@@ -38588,7 +38730,7 @@
     </row>
     <row r="150" spans="1:4" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="44"/>
-      <c r="B150" s="74" t="s">
+      <c r="B150" s="91" t="s">
         <v>195</v>
       </c>
       <c r="C150" s="37"/>
@@ -39486,7 +39628,7 @@
     </row>
     <row r="240" spans="1:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="44"/>
-      <c r="B240" s="74" t="s">
+      <c r="B240" s="91" t="s">
         <v>284</v>
       </c>
       <c r="C240" s="37"/>
@@ -40164,7 +40306,7 @@
     </row>
     <row r="308" spans="1:4" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="44"/>
-      <c r="B308" s="74" t="s">
+      <c r="B308" s="91" t="s">
         <v>352</v>
       </c>
       <c r="C308" s="37"/>
@@ -40382,7 +40524,7 @@
     </row>
     <row r="330" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="44"/>
-      <c r="B330" s="74" t="s">
+      <c r="B330" s="91" t="s">
         <v>374</v>
       </c>
       <c r="C330" s="37"/>
@@ -40760,7 +40902,7 @@
     </row>
     <row r="368" spans="1:4" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="44"/>
-      <c r="B368" s="74" t="s">
+      <c r="B368" s="91" t="s">
         <v>395</v>
       </c>
       <c r="C368" s="37"/>
@@ -40858,7 +41000,7 @@
     </row>
     <row r="378" spans="1:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A378" s="44"/>
-      <c r="B378" s="74" t="s">
+      <c r="B378" s="91" t="s">
         <v>405</v>
       </c>
       <c r="C378" s="37"/>
@@ -40886,7 +41028,7 @@
     </row>
     <row r="381" spans="1:4" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A381" s="44"/>
-      <c r="B381" s="74" t="s">
+      <c r="B381" s="91" t="s">
         <v>408</v>
       </c>
       <c r="C381" s="37"/>
@@ -40934,7 +41076,7 @@
     </row>
     <row r="386" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="44"/>
-      <c r="B386" s="74" t="s">
+      <c r="B386" s="91" t="s">
         <v>413</v>
       </c>
       <c r="C386" s="37"/>
@@ -42202,7 +42344,7 @@
     </row>
     <row r="513" spans="1:4" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A513" s="44"/>
-      <c r="B513" s="74" t="s">
+      <c r="B513" s="91" t="s">
         <v>534</v>
       </c>
       <c r="C513" s="37"/>
@@ -42410,13 +42552,19 @@
     </row>
     <row r="534" spans="1:4" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A534" s="42"/>
-      <c r="B534" s="43"/>
+      <c r="B534" s="91" t="s">
+        <v>555</v>
+      </c>
       <c r="C534" s="37"/>
       <c r="D534" s="37"/>
     </row>
     <row r="535" spans="1:4" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A535" s="44"/>
-      <c r="B535" s="43"/>
+      <c r="A535" s="44" t="n">
+        <v>503.0</v>
+      </c>
+      <c r="B535" s="43" t="s">
+        <v>556</v>
+      </c>
       <c r="C535" s="37"/>
       <c r="D535" s="37"/>
     </row>

</xml_diff>